<commit_message>
finish tel county do file
</commit_message>
<xml_diff>
--- a/rawdata/tel_county_changes.xlsx
+++ b/rawdata/tel_county_changes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbgoodman/Dropbox/Data/tels/rawdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbgoodman/Dropbox/Data/tels/tels-data/rawdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -801,10 +801,10 @@
   <dimension ref="A1:M204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomRight" activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2670,7 +2670,7 @@
         <v>13</v>
       </c>
       <c r="E48">
-        <v>1978</v>
+        <v>1979</v>
       </c>
       <c r="F48">
         <v>1</v>

</xml_diff>